<commit_message>
new ref notes added
</commit_message>
<xml_diff>
--- a/RF Notes.xlsx
+++ b/RF Notes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Institution</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,25 @@
   </si>
   <si>
     <t>Kwon0602In-rich</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In-GaN RLPs
+As the films relax(grow) the indium content increases towards the surface. 
+the effect of strain and composition gradients in the symmetric and asymmetric RLPs of InxGa1-xN
+RBS allows an accurate determination of x free from the effects of strain, with depth resolution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strain and composition distributions in wurtzite InGaNÕGaN layers extracted from x-ray reciprocal space mapping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pereira0201Strain</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -446,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -503,6 +522,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:5" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>